<commit_message>
form form new entiry Created
</commit_message>
<xml_diff>
--- a/public/assets/excels/mainFormDBSchema.xlsx
+++ b/public/assets/excels/mainFormDBSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rc/operantnext/public/assets/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA728CBF-C21E-B54C-8442-1B4A06739BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0197449-45C9-B541-8044-F69C92D6E808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16620" xr2:uid="{4F7C1B77-AED9-674C-B229-9F6D76339967}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>profileImage</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>*Aadhar is required for DigiLoker Certificate</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
   </si>
 </sst>
 </file>
@@ -212,7 +221,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -235,13 +244,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,8 +372,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B6709E-7742-C34A-8B15-0301EFE16DEC}" name="Table3" displayName="Table3" ref="A1:D22" totalsRowShown="0">
-  <autoFilter ref="A1:D22" xr:uid="{09B6709E-7742-C34A-8B15-0301EFE16DEC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B6709E-7742-C34A-8B15-0301EFE16DEC}" name="Table3" displayName="Table3" ref="A1:D23" totalsRowShown="0">
+  <autoFilter ref="A1:D23" xr:uid="{09B6709E-7742-C34A-8B15-0301EFE16DEC}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6538A5A0-22C1-5E40-B102-DCDF54BDDEC2}" name="Entity Nmae" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{794DBCE2-E4B7-4E44-B484-40D985B0C317}" name="Data Type" dataDxfId="2"/>
@@ -658,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23B053D-B694-3848-B980-93E7F27BDA67}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,187 +785,199 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
role vise api login created
</commit_message>
<xml_diff>
--- a/public/assets/excels/mainFormDBSchema.xlsx
+++ b/public/assets/excels/mainFormDBSchema.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rc/operantnext/public/assets/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DD82DA-BFFA-0343-864E-120F213A7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BF24CE-225D-F844-860E-62AEBB3A4C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16620" xr2:uid="{4F7C1B77-AED9-674C-B229-9F6D76339967}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{4F7C1B77-AED9-674C-B229-9F6D76339967}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="user" sheetId="1" r:id="rId1"/>
+    <sheet name="event" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>profileImage</t>
   </si>
@@ -198,6 +198,63 @@
   </si>
   <si>
     <t>Date of birth</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>isPaid</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>registrationUrl</t>
+  </si>
+  <si>
+    <t>location.address</t>
+  </si>
+  <si>
+    <t>location.city</t>
+  </si>
+  <si>
+    <t>location.state</t>
+  </si>
+  <si>
+    <t>location.country</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>organizer</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>attendees</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>PK(Organizer)</t>
+  </si>
+  <si>
+    <t>string[]</t>
+  </si>
+  <si>
+    <t>PK(User)</t>
   </si>
 </sst>
 </file>
@@ -213,15 +270,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -257,19 +320,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -375,10 +496,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B6709E-7742-C34A-8B15-0301EFE16DEC}" name="Table3" displayName="Table3" ref="A1:D23" totalsRowShown="0">
   <autoFilter ref="A1:D23" xr:uid="{09B6709E-7742-C34A-8B15-0301EFE16DEC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6538A5A0-22C1-5E40-B102-DCDF54BDDEC2}" name="Entity Nmae" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{794DBCE2-E4B7-4E44-B484-40D985B0C317}" name="Data Type" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{EAA50B2C-311A-224D-8694-A6AC401D75FF}" name="Label Name" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{7BFFEC96-EF48-BE4A-8393-EB284EECB0B5}" name="Remaks" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6538A5A0-22C1-5E40-B102-DCDF54BDDEC2}" name="Entity Nmae" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{794DBCE2-E4B7-4E44-B484-40D985B0C317}" name="Data Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{EAA50B2C-311A-224D-8694-A6AC401D75FF}" name="Label Name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7BFFEC96-EF48-BE4A-8393-EB284EECB0B5}" name="Remaks" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A81D5CEC-1FAB-E944-B6EF-BDFB6ED4A3C1}" name="Table32" displayName="Table32" ref="A1:B16" totalsRowShown="0">
+  <autoFilter ref="A1:B16" xr:uid="{A81D5CEC-1FAB-E944-B6EF-BDFB6ED4A3C1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4C3B869E-0261-F94C-8E74-636431E41C5F}" name="Entity Nmae" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2339D626-8CD2-4544-AA91-1AAFD6A5C527}" name="Data Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -683,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23B053D-B694-3848-B980-93E7F27BDA67}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C29" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,4 +1119,182 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A600699F-5F78-004D-8E07-E0423E3CF587}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>